<commit_message>
Changes Belschema Template + Onboarding Checklist
PS bericht toegevoegd aan Belschema, Checklist Onboarding spelfouten weggehaald
</commit_message>
<xml_diff>
--- a/Checklists/Onboarding/Checklist Onboarding Stagiair.xlsx
+++ b/Checklists/Onboarding/Checklist Onboarding Stagiair.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shahf\Documents\Stage\Chiefs of IT\Checklist Webshop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shahf\Documents\Stage\Chiefs of IT\Checklists\Onboarding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{13633010-F970-4FAD-AC4D-DB9E9A8E1E16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EAE062F-62F8-47B8-A484-C70A4671197A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{373B8DA4-9724-452B-ABBE-436E107CFBEA}"/>
   </bookViews>
@@ -41,9 +41,6 @@
     <t>Chiefs of IT</t>
   </si>
   <si>
-    <t>Ben je bezig met het aannemen van een nieuwe medewerker? Deze checklist helpt je om het onboardingproces overzichtelijk en effectief te laten verlopen. Het zorgt ervoor dat alle belangrijke stappen – van voorbereiding tot de eerste werkdag – goed zijn geregeld.</t>
-  </si>
-  <si>
     <t>088 - 786 0100</t>
   </si>
   <si>
@@ -56,9 +53,6 @@
     <t>Mutual Non Disclosure Agreement doorgenomen, ingevuld, en ondertekend</t>
   </si>
   <si>
-    <t>Duidelijkheid over eerste werkdag</t>
-  </si>
-  <si>
     <t>Voorbereiden Apparatuur</t>
   </si>
   <si>
@@ -147,6 +141,12 @@
   </si>
   <si>
     <t>Hoeveelheid verwachte stageuren</t>
+  </si>
+  <si>
+    <t>Ben je bezig met het aannemen van een nieuwe stagiair? Deze checklist helpt je om het onboardingproces overzichtelijk en effectief te laten verlopen. Het zorgt ervoor dat alle belangrijke stappen – van voorbereiding tot de eerste werkdag – goed zijn geregeld.</t>
+  </si>
+  <si>
+    <t>Duidelijkheid over eerste stagedag</t>
   </si>
 </sst>
 </file>
@@ -808,8 +808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4EADF5A-1937-485E-8D97-E1F1F19B7514}">
   <dimension ref="A3:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.7"/>
@@ -826,37 +826,37 @@
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A5" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="6"/>
     </row>
     <row r="6" spans="1:4" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="1.5">
       <c r="A6" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.7">
       <c r="C7" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.7">
       <c r="C8" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D8" s="10" t="b">
         <v>0</v>
@@ -864,7 +864,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.7">
       <c r="C9" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D9" s="12" t="b">
         <v>0</v>
@@ -872,7 +872,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.7">
       <c r="C10" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D10" s="12" t="b">
         <v>0</v>
@@ -880,7 +880,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.7">
       <c r="C11" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D11" s="12" t="b">
         <v>0</v>
@@ -888,7 +888,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.7">
       <c r="C12" s="11" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D12" s="12" t="b">
         <v>0</v>
@@ -896,13 +896,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.7">
       <c r="C13" s="13" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D13" s="14"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.7">
       <c r="C14" s="15" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D14" s="16" t="b">
         <v>0</v>
@@ -910,7 +910,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.7">
       <c r="C15" s="15" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D15" s="16" t="b">
         <v>0</v>
@@ -918,7 +918,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.7">
       <c r="C16" s="15" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D16" s="16" t="b">
         <v>0</v>
@@ -926,7 +926,7 @@
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.7">
       <c r="C17" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D17" s="16" t="b">
         <v>0</v>
@@ -934,7 +934,7 @@
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.7">
       <c r="C18" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D18" s="16" t="b">
         <v>0</v>
@@ -942,7 +942,7 @@
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.7">
       <c r="C19" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D19" s="16" t="b">
         <v>0</v>
@@ -950,7 +950,7 @@
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.7">
       <c r="C20" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D20" s="16" t="b">
         <v>0</v>
@@ -958,7 +958,7 @@
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.7">
       <c r="C21" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D21" s="16" t="b">
         <v>0</v>
@@ -966,7 +966,7 @@
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.7">
       <c r="C22" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D22" s="16" t="b">
         <v>0</v>
@@ -974,7 +974,7 @@
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.7">
       <c r="C23" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D23" s="16" t="b">
         <v>0</v>
@@ -982,7 +982,7 @@
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.7">
       <c r="C24" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D24" s="16" t="b">
         <v>0</v>
@@ -990,7 +990,7 @@
     </row>
     <row r="25" spans="3:4" x14ac:dyDescent="0.7">
       <c r="C25" s="15" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D25" s="16" t="b">
         <v>0</v>
@@ -998,13 +998,13 @@
     </row>
     <row r="26" spans="3:4" x14ac:dyDescent="0.7">
       <c r="C26" s="17" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D26" s="18"/>
     </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.7">
       <c r="C27" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D27" s="19" t="b">
         <v>0</v>
@@ -1012,7 +1012,7 @@
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.7">
       <c r="C28" s="15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D28" s="19" t="b">
         <v>0</v>
@@ -1020,7 +1020,7 @@
     </row>
     <row r="29" spans="3:4" x14ac:dyDescent="0.7">
       <c r="C29" s="15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D29" s="19" t="b">
         <v>0</v>
@@ -1028,13 +1028,13 @@
     </row>
     <row r="30" spans="3:4" x14ac:dyDescent="0.7">
       <c r="C30" s="20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D30" s="21"/>
     </row>
     <row r="31" spans="3:4" x14ac:dyDescent="0.7">
       <c r="C31" s="15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D31" s="22" t="b">
         <v>0</v>
@@ -1042,7 +1042,7 @@
     </row>
     <row r="32" spans="3:4" x14ac:dyDescent="0.7">
       <c r="C32" s="15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D32" s="22" t="b">
         <v>0</v>
@@ -1050,7 +1050,7 @@
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.7">
       <c r="C33" s="15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D33" s="22" t="b">
         <v>0</v>
@@ -1058,13 +1058,13 @@
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.7">
       <c r="C34" s="23" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D34" s="24"/>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.7">
       <c r="C35" s="15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D35" s="25" t="b">
         <v>0</v>
@@ -1072,7 +1072,7 @@
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.7">
       <c r="C36" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D36" s="25" t="b">
         <v>0</v>
@@ -1080,7 +1080,7 @@
     </row>
     <row r="37" spans="3:4" x14ac:dyDescent="0.7">
       <c r="C37" s="26" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D37" s="25" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Checklist Stagiair 2.0 + Belschema 3.0
Extra step toegevoegd aan Belschema, 3 extra checks gezet bij Checklist Stagiair
</commit_message>
<xml_diff>
--- a/Checklists/Onboarding/Checklist Onboarding Stagiair.xlsx
+++ b/Checklists/Onboarding/Checklist Onboarding Stagiair.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shahf\Documents\Stage\Chiefs of IT\Checklists\Onboarding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EAE062F-62F8-47B8-A484-C70A4671197A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B607C46-ACE2-4E36-9D61-16648CF05699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{373B8DA4-9724-452B-ABBE-436E107CFBEA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Chiefs of IT</t>
   </si>
@@ -143,10 +143,22 @@
     <t>Hoeveelheid verwachte stageuren</t>
   </si>
   <si>
-    <t>Ben je bezig met het aannemen van een nieuwe stagiair? Deze checklist helpt je om het onboardingproces overzichtelijk en effectief te laten verlopen. Het zorgt ervoor dat alle belangrijke stappen – van voorbereiding tot de eerste werkdag – goed zijn geregeld.</t>
-  </si>
-  <si>
     <t>Duidelijkheid over eerste stagedag</t>
+  </si>
+  <si>
+    <t>Startgesprek met coördinator</t>
+  </si>
+  <si>
+    <t>Tussengesprek met coördinator</t>
+  </si>
+  <si>
+    <t>Eindgesprek met coördinator</t>
+  </si>
+  <si>
+    <t>Ben je bezig met het aannemen van een nieuwe stagiair? Deze checklist helpt je om het onboardingproces overzichtelijk en effectief te laten verlopen. Het zorgt ervoor dat alle belangrijke stappen – van voorbereiding tot de eerste stagedag – goed zijn geregeld.</t>
+  </si>
+  <si>
+    <t>Duidelijkheid over werkzaamheden</t>
   </si>
 </sst>
 </file>
@@ -806,10 +818,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4EADF5A-1937-485E-8D97-E1F1F19B7514}">
-  <dimension ref="A3:D37"/>
+  <dimension ref="A3:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.7"/>
@@ -826,7 +838,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.7">
@@ -888,29 +900,29 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.7">
       <c r="C12" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D12" s="12" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.7">
+      <c r="C14" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="14"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="C14" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="16" t="b">
-        <v>0</v>
-      </c>
+      <c r="D14" s="14"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.7">
       <c r="C15" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D15" s="16" t="b">
         <v>0</v>
@@ -918,31 +930,31 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.7">
       <c r="C16" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.7">
+      <c r="C17" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.7">
-      <c r="C17" s="9" t="s">
+      <c r="D17" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.7">
+      <c r="C18" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.7">
-      <c r="C18" s="11" t="s">
+      <c r="D18" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.7">
+      <c r="C19" s="11" t="s">
         <v>19</v>
-      </c>
-      <c r="D18" s="16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.7">
-      <c r="C19" s="9" t="s">
-        <v>20</v>
       </c>
       <c r="D19" s="16" t="b">
         <v>0</v>
@@ -950,7 +962,7 @@
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.7">
       <c r="C20" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D20" s="16" t="b">
         <v>0</v>
@@ -958,7 +970,7 @@
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.7">
       <c r="C21" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D21" s="16" t="b">
         <v>0</v>
@@ -966,7 +978,7 @@
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.7">
       <c r="C22" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D22" s="16" t="b">
         <v>0</v>
@@ -974,7 +986,7 @@
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.7">
       <c r="C23" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D23" s="16" t="b">
         <v>0</v>
@@ -982,37 +994,37 @@
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.7">
       <c r="C24" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.7">
+      <c r="C25" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.7">
-      <c r="C25" s="15" t="s">
+      <c r="D25" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="3:4" x14ac:dyDescent="0.7">
+      <c r="C26" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.7">
-      <c r="C26" s="17" t="s">
+      <c r="D26" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="3:4" x14ac:dyDescent="0.7">
+      <c r="C27" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D26" s="18"/>
-    </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.7">
-      <c r="C27" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="D27" s="19" t="b">
-        <v>0</v>
-      </c>
+      <c r="D27" s="18"/>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.7">
       <c r="C28" s="15" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="D28" s="19" t="b">
         <v>0</v>
@@ -1020,29 +1032,29 @@
     </row>
     <row r="29" spans="3:4" x14ac:dyDescent="0.7">
       <c r="C29" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="3:4" x14ac:dyDescent="0.7">
+      <c r="C30" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D29" s="19" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.7">
-      <c r="C30" s="20" t="s">
+      <c r="D30" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="3:4" x14ac:dyDescent="0.7">
+      <c r="C31" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D30" s="21"/>
-    </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.7">
-      <c r="C31" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="D31" s="22" t="b">
-        <v>0</v>
-      </c>
+      <c r="D31" s="21"/>
     </row>
     <row r="32" spans="3:4" x14ac:dyDescent="0.7">
       <c r="C32" s="15" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D32" s="22" t="b">
         <v>0</v>
@@ -1050,39 +1062,71 @@
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.7">
       <c r="C33" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" s="22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.7">
+      <c r="C34" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D33" s="22" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.7">
-      <c r="C34" s="23" t="s">
+      <c r="D34" s="22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="3:4" x14ac:dyDescent="0.7">
+      <c r="C35" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D34" s="24"/>
-    </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.7">
-      <c r="C35" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D35" s="25" t="b">
-        <v>0</v>
-      </c>
+      <c r="D35" s="24"/>
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.7">
       <c r="C36" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" s="25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4" x14ac:dyDescent="0.7">
+      <c r="C37" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D36" s="25" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.7">
-      <c r="C37" s="26" t="s">
+      <c r="D37" s="25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="3:4" x14ac:dyDescent="0.7">
+      <c r="C38" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="D37" s="25" t="b">
+      <c r="D38" s="25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="3:4" x14ac:dyDescent="0.7">
+      <c r="C39" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D39" s="25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="3:4" x14ac:dyDescent="0.7">
+      <c r="C40" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D40" s="25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="3:4" x14ac:dyDescent="0.7">
+      <c r="C41" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D41" s="25" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>